<commit_message>
Update variable units and range
- Also included the slider variables
- Made a new screenshot for the variables
</commit_message>
<xml_diff>
--- a/conceptualisation/Variables units and ranges.xlsx
+++ b/conceptualisation/Variables units and ranges.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thomas\Documents\Github\SEN1211-earthquake-project\conceptualisation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DCB4EDF5-8994-4863-A89B-2A6DECAB7487}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36C250D9-AC43-48A0-8E78-49F3CF4BB08B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{3C69A6DE-F24C-4B98-A552-A6CEA12EA266}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
+    <sheet name="Blad2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="158">
   <si>
     <t>Variable</t>
   </si>
@@ -393,6 +394,123 @@
   </si>
   <si>
     <t>Tracks how many residents have recovered inside an ambulance or at home with checking</t>
+  </si>
+  <si>
+    <t>Sliders</t>
+  </si>
+  <si>
+    <t>Earthquake-magnitude</t>
+  </si>
+  <si>
+    <t>Probability-call-112</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>Probability that resident … calls 112 the current tick</t>
+  </si>
+  <si>
+    <t>Amount-ambulances</t>
+  </si>
+  <si>
+    <t>Amount of ambulances</t>
+  </si>
+  <si>
+    <t>Limited to 250 in slider</t>
+  </si>
+  <si>
+    <t>Amount-hospitals</t>
+  </si>
+  <si>
+    <t>Amount of hospitals</t>
+  </si>
+  <si>
+    <t>Limited to 30 in slider</t>
+  </si>
+  <si>
+    <t>Hospital-capacity</t>
+  </si>
+  <si>
+    <t>Hospital-filling-percegate-t0</t>
+  </si>
+  <si>
+    <t>Percentage of hospital capacity that was filled with patients before earthquake</t>
+  </si>
+  <si>
+    <t>Initial-ambulance-search-radius</t>
+  </si>
+  <si>
+    <t>0-1900</t>
+  </si>
+  <si>
+    <t>What is the radius in which the ambulance will initially search for a patient</t>
+  </si>
+  <si>
+    <t>Percentage-concrete-buildings</t>
+  </si>
+  <si>
+    <t>High-damage-road-bloacked-chance</t>
+  </si>
+  <si>
+    <t>Collapsed-road-blocked-chance</t>
+  </si>
+  <si>
+    <t>Max-concurrent-calls</t>
+  </si>
+  <si>
+    <t>Amount of calls</t>
+  </si>
+  <si>
+    <t>Only works if call-limit is in place. Limited to 100 in slider</t>
+  </si>
+  <si>
+    <t>Average-call-time</t>
+  </si>
+  <si>
+    <t>Only works if call-limit is in place. Limited to 15 in slider</t>
+  </si>
+  <si>
+    <t>Amount-drones</t>
+  </si>
+  <si>
+    <t>Amount of drones</t>
+  </si>
+  <si>
+    <t>Drone-speed</t>
+  </si>
+  <si>
+    <t>m/s</t>
+  </si>
+  <si>
+    <t>Limited to 25 in slider</t>
+  </si>
+  <si>
+    <t>One patch is appr. 10 by 10 meters. Limited to 1 in slider</t>
+  </si>
+  <si>
+    <t>Drone-view-radius</t>
+  </si>
+  <si>
+    <t>Similarlyt to initial-ambulances-search-radius 1900 patchs is the max distance in model</t>
+  </si>
+  <si>
+    <t>Drone-range</t>
+  </si>
+  <si>
+    <t>Minutes (1 tick is 1 minute)</t>
+  </si>
+  <si>
+    <t>Limited to 90 in slider</t>
+  </si>
+  <si>
+    <t>Ambulance-reroute-frequency</t>
+  </si>
+  <si>
+    <t>Ticks</t>
+  </si>
+  <si>
+    <t>Ticks before rerouting of ambulance happens. Limited to 100 in slider</t>
   </si>
 </sst>
 </file>
@@ -748,10 +866,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{437E2068-B3EB-4E53-A89A-C3DB54A1A3DE}">
-  <dimension ref="A1:F46"/>
+  <dimension ref="A1:F64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D52" sqref="D52"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D70" sqref="D70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1410,7 +1528,299 @@
         <v>118</v>
       </c>
     </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>119</v>
+      </c>
+      <c r="B48" t="s">
+        <v>120</v>
+      </c>
+      <c r="C48" t="s">
+        <v>7</v>
+      </c>
+      <c r="D48">
+        <v>0</v>
+      </c>
+      <c r="E48" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="49" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B49" t="s">
+        <v>121</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D49" s="1">
+        <v>100</v>
+      </c>
+      <c r="E49" t="s">
+        <v>122</v>
+      </c>
+      <c r="F49" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="50" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B50" t="s">
+        <v>124</v>
+      </c>
+      <c r="C50" t="s">
+        <v>25</v>
+      </c>
+      <c r="D50" t="s">
+        <v>52</v>
+      </c>
+      <c r="E50" t="s">
+        <v>125</v>
+      </c>
+      <c r="F50" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="51" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B51" t="s">
+        <v>127</v>
+      </c>
+      <c r="C51" t="s">
+        <v>25</v>
+      </c>
+      <c r="D51" t="s">
+        <v>52</v>
+      </c>
+      <c r="E51" t="s">
+        <v>128</v>
+      </c>
+      <c r="F51" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="52" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B52" t="s">
+        <v>130</v>
+      </c>
+      <c r="C52" t="s">
+        <v>25</v>
+      </c>
+      <c r="D52" t="s">
+        <v>52</v>
+      </c>
+      <c r="E52" t="s">
+        <v>58</v>
+      </c>
+      <c r="F52" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="53" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B53" t="s">
+        <v>131</v>
+      </c>
+      <c r="C53" t="s">
+        <v>85</v>
+      </c>
+      <c r="D53">
+        <v>0</v>
+      </c>
+      <c r="E53" t="s">
+        <v>122</v>
+      </c>
+      <c r="F53" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="54" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B54" t="s">
+        <v>133</v>
+      </c>
+      <c r="C54" t="s">
+        <v>134</v>
+      </c>
+      <c r="D54" t="s">
+        <v>30</v>
+      </c>
+      <c r="E54" t="s">
+        <v>53</v>
+      </c>
+      <c r="F54" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="55" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B55" t="s">
+        <v>136</v>
+      </c>
+      <c r="C55" t="s">
+        <v>85</v>
+      </c>
+      <c r="D55">
+        <v>100</v>
+      </c>
+      <c r="E55" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="56" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B56" t="s">
+        <v>137</v>
+      </c>
+      <c r="C56" t="s">
+        <v>85</v>
+      </c>
+      <c r="D56">
+        <v>0</v>
+      </c>
+      <c r="E56" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="57" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B57" t="s">
+        <v>138</v>
+      </c>
+      <c r="C57" t="s">
+        <v>85</v>
+      </c>
+      <c r="D57">
+        <v>0</v>
+      </c>
+      <c r="E57" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="58" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B58" t="s">
+        <v>139</v>
+      </c>
+      <c r="C58" t="s">
+        <v>25</v>
+      </c>
+      <c r="D58" t="s">
+        <v>52</v>
+      </c>
+      <c r="E58" t="s">
+        <v>140</v>
+      </c>
+      <c r="F58" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="59" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B59" t="s">
+        <v>142</v>
+      </c>
+      <c r="C59" t="s">
+        <v>25</v>
+      </c>
+      <c r="D59">
+        <v>0</v>
+      </c>
+      <c r="E59" t="s">
+        <v>26</v>
+      </c>
+      <c r="F59" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="60" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B60" t="s">
+        <v>144</v>
+      </c>
+      <c r="C60" t="s">
+        <v>25</v>
+      </c>
+      <c r="D60" t="s">
+        <v>52</v>
+      </c>
+      <c r="E60" t="s">
+        <v>145</v>
+      </c>
+      <c r="F60" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="61" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B61" t="s">
+        <v>146</v>
+      </c>
+      <c r="C61" t="s">
+        <v>25</v>
+      </c>
+      <c r="D61" t="s">
+        <v>52</v>
+      </c>
+      <c r="E61" t="s">
+        <v>147</v>
+      </c>
+      <c r="F61" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="62" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B62" t="s">
+        <v>150</v>
+      </c>
+      <c r="C62" t="s">
+        <v>134</v>
+      </c>
+      <c r="D62">
+        <v>1900</v>
+      </c>
+      <c r="E62" t="s">
+        <v>53</v>
+      </c>
+      <c r="F62" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="63" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B63" t="s">
+        <v>152</v>
+      </c>
+      <c r="C63" t="s">
+        <v>25</v>
+      </c>
+      <c r="D63" t="s">
+        <v>52</v>
+      </c>
+      <c r="E63" t="s">
+        <v>153</v>
+      </c>
+      <c r="F63" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="64" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B64" t="s">
+        <v>155</v>
+      </c>
+      <c r="C64" t="s">
+        <v>25</v>
+      </c>
+      <c r="D64">
+        <v>0</v>
+      </c>
+      <c r="E64" t="s">
+        <v>156</v>
+      </c>
+      <c r="F64" t="s">
+        <v>157</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FDB7B1A-885E-4B10-B68F-B332542DB730}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>